<commit_message>
added a back ground image for the strat page, and started writing out test cases, also working on the degien of the grid page, and working on the gird, going to be spending the next 2hrs on it, and then have to study for applied netowrking exam
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaroncronnelly/Documents/GitHub/MaterMinds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C953A2C-7948-7C49-A33D-69E151F84656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF20BC7-C430-3140-BFAC-E8A7B293E865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{0DAC86A6-B007-2D4A-846E-165DFFA658DA}"/>
+    <workbookView xWindow="29140" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{0DAC86A6-B007-2D4A-846E-165DFFA658DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,47 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>Case's</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Expexeped outcome</t>
+  </si>
+  <si>
+    <t>True outcome</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Clicking Start Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They game should move to the game screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goes to game screen </t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicking on rules button </t>
+  </si>
+  <si>
+    <t>Should display a alert explaing the aleart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show user rules and how to play </t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -86,7 +127,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -374,7 +415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -382,12 +423,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77086B28-B0BD-CC42-B896-4281C7044AB7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated test case, also began work on getting the check answer method to work, once done, then random genterated color code, can be made, and then move on two the abilty to itterate each time the use get and answer wrong
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaroncronnelly/Documents/GitHub/MaterMinds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF20BC7-C430-3140-BFAC-E8A7B293E865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483A2CE1-867D-B14B-B6C1-C32A41AE06F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29140" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{0DAC86A6-B007-2D4A-846E-165DFFA658DA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{0DAC86A6-B007-2D4A-846E-165DFFA658DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Case's</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t xml:space="preserve">Show user rules and how to play </t>
+  </si>
+  <si>
+    <t>Clicking on boxview color</t>
+  </si>
+  <si>
+    <t>should change the color depending on how many times the user clicks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cycles throught colors each time user clicks </t>
   </si>
 </sst>
 </file>
@@ -423,18 +432,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77086B28-B0BD-CC42-B896-4281C7044AB7}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
-    <col min="3" max="3" width="44.5" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -488,6 +498,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
working on grid, Got the grid working to an extent that the user, can only acess the grid that they are on. Currently working on tyring to get the inputreplyGrid to work, but having truble with it as only the first col is updating, and the rest arnt
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaroncronnelly/Documents/GitHub/MaterMinds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483A2CE1-867D-B14B-B6C1-C32A41AE06F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED109DD-FC17-4D43-9AF5-71AE6BDF1DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{0DAC86A6-B007-2D4A-846E-165DFFA658DA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Case's</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t xml:space="preserve">cycles throught colors each time user clicks </t>
+  </si>
+  <si>
+    <t>clicking on boxview cheat pertection</t>
+  </si>
+  <si>
+    <t>user can only click on the first row at the start and then work their way down the grid only allowed to click on theat curretn row they are on</t>
+  </si>
+  <si>
+    <t>check pertechion works</t>
   </si>
 </sst>
 </file>
@@ -432,17 +441,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77086B28-B0BD-CC42-B896-4281C7044AB7}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -515,6 +524,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
having trouble on trying to get the pegGrid to update properly
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaroncronnelly/Documents/GitHub/MaterMinds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED109DD-FC17-4D43-9AF5-71AE6BDF1DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83524D1-CE24-F74C-AB0E-6F8C8D255C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{0DAC86A6-B007-2D4A-846E-165DFFA658DA}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
final update before, submission, tested on phone, working, but some lag
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaroncronnelly/Documents/GitHub/MaterMinds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83524D1-CE24-F74C-AB0E-6F8C8D255C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1909CF80-2A57-5744-A242-D416C3BFE595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{0DAC86A6-B007-2D4A-846E-165DFFA658DA}"/>
+    <workbookView xWindow="28980" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{0DAC86A6-B007-2D4A-846E-165DFFA658DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Case's</t>
   </si>
@@ -90,6 +90,24 @@
   </si>
   <si>
     <t>check pertechion works</t>
+  </si>
+  <si>
+    <t>Random color code</t>
+  </si>
+  <si>
+    <t>fucntion should creatse a random 4 color code</t>
+  </si>
+  <si>
+    <t>fucntion does create a for color code</t>
+  </si>
+  <si>
+    <t>Phone test</t>
+  </si>
+  <si>
+    <t>all above test should work on phone</t>
+  </si>
+  <si>
+    <t>working as expected, althoug some lag</t>
   </si>
 </sst>
 </file>
@@ -441,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77086B28-B0BD-CC42-B896-4281C7044AB7}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,6 +559,40 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>